<commit_message>
update excel games column
</commit_message>
<xml_diff>
--- a/scores_example.xlsx
+++ b/scores_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dartr\OneDrive\Documents\github\ScoreTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC1D5CF-16B8-4B18-8062-78E5234008FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{543CF88C-6A08-48C9-8623-5CA6D1D25C57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="21">
   <si>
     <t>Games</t>
   </si>
@@ -92,6 +91,9 @@
   </si>
   <si>
     <t>FCC</t>
+  </si>
+  <si>
+    <t>FCC-GAC</t>
   </si>
 </sst>
 </file>
@@ -412,7 +414,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -455,8 +457,8 @@
       <c r="L1" s="3"/>
     </row>
     <row r="2" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="7">
-        <v>1</v>
+      <c r="A2" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>18</v>
@@ -698,8 +700,8 @@
       <c r="L11" s="3"/>
     </row>
     <row r="12" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>2</v>
+      <c r="A12" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>18</v>

</xml_diff>